<commit_message>
add write data to equipment file
</commit_message>
<xml_diff>
--- a/eq_log/80001111.xlsx
+++ b/eq_log/80001111.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -38,10 +38,28 @@
     <t>Аплікатор</t>
   </si>
   <si>
+    <t>24/01/2018</t>
+  </si>
+  <si>
+    <t>3012</t>
+  </si>
+  <si>
+    <t>write data</t>
+  </si>
+  <si>
+    <t>123456987</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>Пошкодження поверхні контакту</t>
+  </si>
+  <si>
+    <t>123698547</t>
+  </si>
+  <si>
     <t>**</t>
-  </si>
-  <si>
-    <t>Пошкодження поверхні контакту</t>
   </si>
   <si>
     <t>розшифровка</t>
@@ -208,9 +226,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
@@ -497,50 +523,48 @@
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf borderId="0" fillId="6" fontId="6" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="4" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="5" fontId="1" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="2" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="8" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -581,12 +605,17 @@
     <xf applyAlignment="1" borderId="11" fillId="10" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="7" fillId="6" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf applyAlignment="1" borderId="3" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="7" fillId="6" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -891,7 +920,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -908,63 +937,211 @@
       <c r="A1" s="32" t="n">
         <v>80001111</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row customHeight="1" ht="29.45" r="2" s="34" spans="1:8">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="11" t="n"/>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="10" t="n"/>
+      <c r="G2" s="36" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="9" t="n"/>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="2" t="n"/>
+      <c r="E3" s="2">
+        <f>D3-D2</f>
+        <v/>
+      </c>
+      <c r="F3" s="11" t="n"/>
+      <c r="G3" s="33" t="n"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10" t="n"/>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="3" t="n"/>
-      <c r="E3" s="3" t="n"/>
-      <c r="F3" s="12" t="n"/>
-      <c r="G3" s="33" t="n"/>
-    </row>
-    <row r="4" spans="1:8"/>
-    <row r="5" spans="1:8"/>
-    <row r="6" spans="1:8"/>
-    <row r="7" spans="1:8"/>
-    <row r="8" spans="1:8"/>
-    <row r="9" spans="1:8"/>
-    <row r="10" spans="1:8"/>
-    <row r="11" spans="1:8"/>
-    <row r="12" spans="1:8"/>
-    <row r="13" spans="1:8"/>
-    <row r="14" spans="1:8"/>
-    <row r="15" spans="1:8"/>
-    <row r="16" spans="1:8"/>
-    <row r="17" spans="1:8"/>
-    <row r="18" spans="1:8"/>
-    <row r="19" spans="1:8"/>
-    <row r="20" spans="1:8"/>
-    <row r="21" spans="1:8"/>
-    <row r="22" spans="1:8"/>
-    <row r="23" spans="1:8"/>
-    <row r="24" spans="1:8"/>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2">
+        <f>D4-D3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2">
+        <f>D5-D4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2">
+        <f>D6-D5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2">
+        <f>D7-D6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2">
+        <f>D8-D7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="E9" s="2">
+        <f>D9-D8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="E10" s="2">
+        <f>D10-D9</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="E11" s="2">
+        <f>D11-D10</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="E12" s="2">
+        <f>D12-D11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="E13" s="2">
+        <f>D13-D12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="E14" s="2">
+        <f>D14-D13</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="E15" s="2">
+        <f>D15-D14</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="E16" s="2">
+        <f>D16-D15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="E17" s="2">
+        <f>D17-D16</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="E18" s="2">
+        <f>D18-D17</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="E19" s="2">
+        <f>D19-D18</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="E20" s="2">
+        <f>D20-D19</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="E21" s="2">
+        <f>D21-D20</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="E22" s="2">
+        <f>D22-D21</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="E23" s="2">
+        <f>D23-D22</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="E24" s="2">
+        <f>D24-D23</f>
+        <v/>
+      </c>
+    </row>
     <row r="25" spans="1:8"/>
     <row r="26" spans="1:8"/>
     <row r="27" spans="1:8"/>
@@ -1000,310 +1177,310 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="14" t="s">
-        <v>8</v>
+      <c r="A1" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="D1" s="35" t="n"/>
       <c r="E1" s="35" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="2" s="34" spans="1:5" thickBot="1">
-      <c r="A2" s="14" t="s">
-        <v>10</v>
+      <c r="A2" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>13</v>
+      <c r="A3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>15</v>
+      <c r="A4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>17</v>
+      <c r="A5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>19</v>
+      <c r="E6" s="24" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>21</v>
+      <c r="A7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>23</v>
+      <c r="A8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>25</v>
+      <c r="A9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>27</v>
+      <c r="A10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>29</v>
+      <c r="A11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>31</v>
+      <c r="A12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>33</v>
+      <c r="A13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>35</v>
+      <c r="A14" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>37</v>
+      <c r="A15" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>39</v>
+      <c r="A16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>45</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="17" s="34" spans="1:5" thickBot="1">
-      <c r="A17" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="28" t="s">
-        <v>42</v>
+      <c r="A17" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="D18" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>44</v>
+      <c r="D18" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="D19" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>45</v>
+      <c r="D19" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="D20" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>46</v>
+      <c r="D20" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="D21" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>47</v>
+      <c r="D21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="D22" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>48</v>
+      <c r="D22" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="23" s="34" spans="1:5" thickBot="1">
-      <c r="D23" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="28" t="s">
+      <c r="D23" s="20" t="s">
         <v>49</v>
       </c>
+      <c r="E23" s="26" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="D24" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>51</v>
+      <c r="D24" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="D25" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="26" t="s">
-        <v>52</v>
+      <c r="D25" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="D26" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="26" t="s">
-        <v>53</v>
+      <c r="D26" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>59</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="27" s="34" spans="1:5" thickBot="1">
-      <c r="D27" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>54</v>
+      <c r="D27" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="D28" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>56</v>
+      <c r="D28" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="D29" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="E29" s="26" t="s">
-        <v>57</v>
+      <c r="D29" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="D30" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="E30" s="26" t="s">
-        <v>58</v>
+      <c r="D30" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="D31" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>59</v>
+      <c r="D31" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="D32" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" s="26" t="s">
-        <v>60</v>
+      <c r="D32" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="33" s="34" spans="1:5" thickBot="1">
-      <c r="D33" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E33" s="28" t="s">
+      <c r="D33" s="29" t="s">
         <v>61</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first step to OOP, not finishid
</commit_message>
<xml_diff>
--- a/eq_log/80001111.xlsx
+++ b/eq_log/80001111.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -59,6 +59,15 @@
     <t>123698547</t>
   </si>
   <si>
+    <t>30/01/2018</t>
+  </si>
+  <si>
+    <t>Обладнання не вмикається / не продукує виріб</t>
+  </si>
+  <si>
+    <t>45698723</t>
+  </si>
+  <si>
     <t>**</t>
   </si>
   <si>
@@ -153,9 +162,6 @@
   </si>
   <si>
     <t>заміна ременів проводопротягувача</t>
-  </si>
-  <si>
-    <t>Обладнання не вмикається / не продукує виріб</t>
   </si>
   <si>
     <t>принтер</t>
@@ -1041,12 +1047,24 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
       <c r="E8" s="2">
         <f>D8-D7</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
       <c r="E9" s="2">
         <f>D9-D8</f>
         <v/>
@@ -1182,305 +1200,305 @@
       </c>
       <c r="D1" s="35" t="n"/>
       <c r="E1" s="35" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="2" s="34" spans="1:5" thickBot="1">
       <c r="A2" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="12" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="12" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="17" s="34" spans="1:5" thickBot="1">
       <c r="A17" s="13" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="D18" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="D19" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="D20" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="D21" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="D22" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="23" s="34" spans="1:5" thickBot="1">
       <c r="D23" s="20" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="D24" s="21" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="D25" s="23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="D26" s="23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="27" s="34" spans="1:5" thickBot="1">
       <c r="D27" s="25" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="D28" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="D29" s="28" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="D30" s="28" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="D31" s="28" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="D32" s="28" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="33" s="34" spans="1:5" thickBot="1">
       <c r="D33" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoring. clean print lines
</commit_message>
<xml_diff>
--- a/eq_log/80001111.xlsx
+++ b/eq_log/80001111.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -77,6 +77,15 @@
     <t>31/01/2018</t>
   </si>
   <si>
+    <t>06/02/2018</t>
+  </si>
+  <si>
+    <t>Зазубрини в місті відрізу контакту</t>
+  </si>
+  <si>
+    <t>22222222222222</t>
+  </si>
+  <si>
     <t>**</t>
   </si>
   <si>
@@ -105,9 +114,6 @@
   </si>
   <si>
     <t>електрична поломка</t>
-  </si>
-  <si>
-    <t>Зазубрини в місті відрізу контакту</t>
   </si>
   <si>
     <t>людський фактор</t>
@@ -1107,12 +1113,24 @@
       <c r="A11" t="s">
         <v>20</v>
       </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
       <c r="E11" s="2">
         <f>D11-D10</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
       <c r="E12" s="2">
         <f>D12-D11</f>
         <v/>
@@ -1227,89 +1245,89 @@
       </c>
       <c r="D1" s="35" t="n"/>
       <c r="E1" s="35" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="2" s="34" spans="1:5" thickBot="1">
       <c r="A2" s="12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="12" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1317,76 +1335,76 @@
         <v>17</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="17" s="34" spans="1:5" thickBot="1">
@@ -1394,138 +1412,138 @@
         <v>15</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="D18" s="18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="D19" s="19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="D20" s="19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="D21" s="19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="D22" s="19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="23" s="34" spans="1:5" thickBot="1">
       <c r="D23" s="20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="D24" s="21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="D25" s="23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="D26" s="23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="27" s="34" spans="1:5" thickBot="1">
       <c r="D27" s="25" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="D28" s="27" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="D29" s="28" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="D30" s="28" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="D31" s="28" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="D32" s="28" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="33" s="34" spans="1:5" thickBot="1">
       <c r="D33" s="29" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>